<commit_message>
re doing with the right dB gain
</commit_message>
<xml_diff>
--- a/Hydrophones/Calibration/ManualRockMovements-1/mov1_calibration_curve.xlsx
+++ b/Hydrophones/Calibration/ManualRockMovements-1/mov1_calibration_curve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Hydrophones\Calibration\ManualRockMovements-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Hydrophones\Calibration\ManualRockMovements-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6866379B-ABA3-47E8-8EB8-531D6369F628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F290BE-B746-463D-B45A-3EDAAEFFB123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>Size (mm)</t>
   </si>
   <si>
-    <t>Env Max A</t>
-  </si>
-  <si>
     <t>Aprox Time Start</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>end_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Env Max A </t>
   </si>
 </sst>
 </file>
@@ -274,7 +274,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -311,8 +311,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.38383558452060335"/>
-                  <c:y val="-8.0484419854682937E-2"/>
+                  <c:x val="-0.34043967364204736"/>
+                  <c:y val="-6.454110826256193E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -433,76 +433,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.59</c:v>
+                  <c:v>7.0800000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26</c:v>
+                  <c:v>2.5700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74</c:v>
+                  <c:v>7.0800000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>3.7100000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2</c:v>
+                  <c:v>2.6100000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2</c:v>
+                  <c:v>2.8400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.21</c:v>
+                  <c:v>2.7799999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33</c:v>
+                  <c:v>4.4900000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.21</c:v>
+                  <c:v>2.8799999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.18</c:v>
+                  <c:v>2.3199999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1</c:v>
+                  <c:v>1.4800000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.33</c:v>
+                  <c:v>4.07E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>1.8100000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.11</c:v>
+                  <c:v>1.4800000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.01</c:v>
+                  <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>9.9000000000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.03</c:v>
+                  <c:v>4.5999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.04</c:v>
+                  <c:v>5.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>1.06E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.04</c:v>
+                  <c:v>5.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.04</c:v>
+                  <c:v>5.1000000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.01</c:v>
+                  <c:v>1.8E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.02</c:v>
+                  <c:v>2.2000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.03</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -510,7 +510,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FAB6-4F99-BA73-E5CB745AC1A1}"/>
+              <c16:uniqueId val="{00000001-29DC-43D6-9D7E-2BF6B7887A94}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1377,26 +1377,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
+      <xdr:colOff>487680</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>109536</xdr:rowOff>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>160974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBA5BC6B-7FFA-7404-10B4-6C5ADDF9CCC6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{308EE4C1-EB4A-4103-8986-D8712A8C1056}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1678,22 +1680,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1701,22 +1703,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>167</v>
       </c>
@@ -1730,25 +1732,25 @@
         <v>48</v>
       </c>
       <c r="E2" s="1">
-        <v>0.59</v>
+        <v>7.0800000000000002E-2</v>
       </c>
       <c r="G2" s="1">
         <f>D2-C2</f>
         <v>7</v>
       </c>
       <c r="H2" s="1">
-        <f>C3-D2</f>
+        <f t="shared" ref="H2:H24" si="0">C3-D2</f>
         <v>32</v>
       </c>
       <c r="J2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K2">
         <f>AVERAGE(H2:H24)</f>
         <v>34.347826086956523</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>6</v>
       </c>
@@ -1762,18 +1764,18 @@
         <v>90</v>
       </c>
       <c r="E3" s="1">
-        <v>0.26</v>
+        <v>2.5700000000000001E-2</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G25" si="0">D3-C3</f>
+        <f t="shared" ref="G3:G25" si="1">D3-C3</f>
         <v>10</v>
       </c>
       <c r="H3" s="1">
-        <f>C4-D3</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -1787,18 +1789,18 @@
         <v>125</v>
       </c>
       <c r="E4" s="1">
-        <v>0.74</v>
+        <v>7.0800000000000002E-2</v>
       </c>
       <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H4" s="1">
-        <f>C5-D4</f>
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>168</v>
       </c>
@@ -1812,18 +1814,18 @@
         <v>160</v>
       </c>
       <c r="E5" s="1">
-        <v>0.28999999999999998</v>
+        <v>3.7100000000000001E-2</v>
       </c>
       <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H5" s="1">
-        <f>C6-D5</f>
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>150</v>
       </c>
@@ -1837,18 +1839,18 @@
         <v>199</v>
       </c>
       <c r="E6" s="1">
-        <v>0.2</v>
+        <v>2.6100000000000002E-2</v>
       </c>
       <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H6" s="1">
-        <f>C7-D6</f>
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>11</v>
       </c>
@@ -1862,18 +1864,18 @@
         <v>234</v>
       </c>
       <c r="E7" s="1">
-        <v>0.2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H7" s="1">
-        <f>C8-D7</f>
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>22</v>
       </c>
@@ -1887,18 +1889,18 @@
         <v>275</v>
       </c>
       <c r="E8" s="1">
-        <v>0.21</v>
+        <v>2.7799999999999998E-2</v>
       </c>
       <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H8" s="1">
-        <f>C9-D8</f>
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>152</v>
       </c>
@@ -1912,18 +1914,18 @@
         <v>320</v>
       </c>
       <c r="E9" s="1">
-        <v>0.33</v>
+        <v>4.4900000000000002E-2</v>
       </c>
       <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H9" s="1">
-        <f>C10-D9</f>
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>12</v>
       </c>
@@ -1937,18 +1939,18 @@
         <v>360</v>
       </c>
       <c r="E10" s="1">
-        <v>0.21</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H10" s="1">
-        <f>C11-D10</f>
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>96</v>
       </c>
@@ -1962,18 +1964,18 @@
         <v>400</v>
       </c>
       <c r="E11" s="1">
-        <v>0.18</v>
+        <v>2.3199999999999998E-2</v>
       </c>
       <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H11" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H11" s="1">
-        <f>C12-D11</f>
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>101</v>
       </c>
@@ -1987,18 +1989,18 @@
         <v>438</v>
       </c>
       <c r="E12" s="1">
-        <v>0.1</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H12" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H12" s="1">
-        <f>C13-D12</f>
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>24</v>
       </c>
@@ -2012,18 +2014,18 @@
         <v>478</v>
       </c>
       <c r="E13" s="1">
-        <v>0.33</v>
+        <v>4.07E-2</v>
       </c>
       <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H13" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H13" s="1">
-        <f>C14-D13</f>
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>107</v>
       </c>
@@ -2037,18 +2039,18 @@
         <v>520</v>
       </c>
       <c r="E14" s="1">
-        <v>0.14000000000000001</v>
+        <v>1.8100000000000002E-2</v>
       </c>
       <c r="G14" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H14" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H14" s="1">
-        <f>C15-D14</f>
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>162</v>
       </c>
@@ -2062,18 +2064,18 @@
         <v>560</v>
       </c>
       <c r="E15" s="1">
-        <v>0.11</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="G15" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H15" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H15" s="1">
-        <f>C16-D15</f>
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>159</v>
       </c>
@@ -2087,18 +2089,18 @@
         <v>610</v>
       </c>
       <c r="E16" s="1">
-        <v>0.01</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H16" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="H16" s="1">
-        <f>C17-D16</f>
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>35</v>
       </c>
@@ -2112,18 +2114,18 @@
         <v>648</v>
       </c>
       <c r="E17" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>9.9000000000000008E-3</v>
       </c>
       <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H17" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H17" s="1">
-        <f>C18-D17</f>
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>69</v>
       </c>
@@ -2137,18 +2139,18 @@
         <v>689</v>
       </c>
       <c r="E18" s="1">
-        <v>0.03</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H18" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H18" s="1">
-        <f>C19-D18</f>
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>85</v>
       </c>
@@ -2162,18 +2164,18 @@
         <v>736</v>
       </c>
       <c r="E19" s="1">
-        <v>0.04</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="G19" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H19" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H19" s="1">
-        <f>C20-D19</f>
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>61</v>
       </c>
@@ -2187,18 +2189,18 @@
         <v>788</v>
       </c>
       <c r="E20" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>1.06E-2</v>
       </c>
       <c r="G20" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H20" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H20" s="1">
-        <f>C21-D20</f>
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>52</v>
       </c>
@@ -2212,18 +2214,18 @@
         <v>825</v>
       </c>
       <c r="E21" s="1">
-        <v>0.04</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="G21" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H21" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H21" s="1">
-        <f>C22-D21</f>
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>165</v>
       </c>
@@ -2237,18 +2239,18 @@
         <v>875</v>
       </c>
       <c r="E22" s="1">
-        <v>0.04</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="G22" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H22" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H22" s="1">
-        <f>C23-D22</f>
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>166</v>
       </c>
@@ -2262,18 +2264,18 @@
         <v>930</v>
       </c>
       <c r="E23" s="1">
-        <v>0.01</v>
+        <v>1.8E-3</v>
       </c>
       <c r="G23" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H23" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H23" s="1">
-        <f>C24-D23</f>
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>53</v>
       </c>
@@ -2287,18 +2289,18 @@
         <v>985</v>
       </c>
       <c r="E24" s="1">
-        <v>0.02</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="G24" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H24" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="H24" s="1">
-        <f>C25-D24</f>
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45</v>
       </c>
@@ -2312,10 +2314,10 @@
         <v>1030</v>
       </c>
       <c r="E25" s="1">
-        <v>0.03</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="H25" s="1"/>
@@ -2334,24 +2336,24 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>167</v>
       </c>
@@ -2362,7 +2364,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>6</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>168</v>
       </c>
@@ -2395,7 +2397,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>150</v>
       </c>
@@ -2406,7 +2408,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>11</v>
       </c>
@@ -2417,7 +2419,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>22</v>
       </c>
@@ -2428,7 +2430,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>152</v>
       </c>
@@ -2439,7 +2441,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>12</v>
       </c>
@@ -2450,7 +2452,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>96</v>
       </c>
@@ -2461,7 +2463,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>101</v>
       </c>
@@ -2472,7 +2474,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>24</v>
       </c>
@@ -2483,7 +2485,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>107</v>
       </c>
@@ -2494,7 +2496,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>162</v>
       </c>
@@ -2505,7 +2507,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>159</v>
       </c>
@@ -2516,7 +2518,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>35</v>
       </c>
@@ -2527,7 +2529,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>69</v>
       </c>
@@ -2538,7 +2540,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>85</v>
       </c>
@@ -2549,7 +2551,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>61</v>
       </c>
@@ -2560,7 +2562,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>52</v>
       </c>
@@ -2571,7 +2573,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>165</v>
       </c>
@@ -2582,7 +2584,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>166</v>
       </c>
@@ -2593,7 +2595,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>53</v>
       </c>
@@ -2604,7 +2606,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
manual rock mov - microphone
</commit_message>
<xml_diff>
--- a/Hydrophones/Calibration/ManualRockMovements-1/mov1_calibration_curve.xlsx
+++ b/Hydrophones/Calibration/ManualRockMovements-1/mov1_calibration_curve.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Hydrophones\Calibration\ManualRockMovements-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F290BE-B746-463D-B45A-3EDAAEFFB123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E51FE61-EC7D-4045-B64B-90704AA31749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="csv for code" sheetId="2" r:id="rId2"/>
+    <sheet name="Impact Pipe" sheetId="1" r:id="rId1"/>
+    <sheet name="Microphone" sheetId="4" r:id="rId2"/>
+    <sheet name="csv for code (pipe)" sheetId="2" r:id="rId3"/>
+    <sheet name="csv for code (mic)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Particle #</t>
   </si>
@@ -70,6 +72,15 @@
   </si>
   <si>
     <t xml:space="preserve">Env Max A </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Max A </t>
+  </si>
+  <si>
+    <t>Env Max A</t>
+  </si>
+  <si>
+    <t>Raw Max A</t>
   </si>
 </sst>
 </file>
@@ -273,6 +284,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Envelope</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -285,11 +299,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -299,7 +313,7 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -311,13 +325,18 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.34043967364204736"/>
-                  <c:y val="-6.454110826256193E-2"/>
+                  <c:x val="-0.3824709704714141"/>
+                  <c:y val="-9.1234101696918882E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="20000"/>
+                    <a:lumOff val="80000"/>
+                  </a:schemeClr>
+                </a:solidFill>
                 <a:ln>
                   <a:noFill/>
                 </a:ln>
@@ -347,10 +366,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:f>'Impact Pipe'!$B$2:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>128</c:v>
                 </c:pt>
@@ -428,69 +447,69 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$25</c:f>
+              <c:f>'Impact Pipe'!$F$2:$F$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>7.0800000000000002E-2</c:v>
+                  <c:v>8.3199999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5700000000000001E-2</c:v>
+                  <c:v>3.7100000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0800000000000002E-2</c:v>
+                  <c:v>0.10489999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7100000000000001E-2</c:v>
+                  <c:v>4.0300000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6100000000000002E-2</c:v>
+                  <c:v>2.86E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.8400000000000002E-2</c:v>
+                  <c:v>2.86E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7799999999999998E-2</c:v>
+                  <c:v>3.0099999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4900000000000002E-2</c:v>
+                  <c:v>4.6800000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8799999999999999E-2</c:v>
+                  <c:v>2.9499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3199999999999998E-2</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.4800000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.07E-2</c:v>
+                  <c:v>4.5900000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.8100000000000002E-2</c:v>
+                  <c:v>1.9800000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.4800000000000001E-2</c:v>
+                  <c:v>1.54E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.9000000000000008E-3</c:v>
+                  <c:v>1.03E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.5999999999999999E-3</c:v>
+                  <c:v>4.7000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.4000000000000003E-3</c:v>
+                  <c:v>5.8999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1.06E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.4000000000000003E-3</c:v>
+                  <c:v>6.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>5.1000000000000004E-3</c:v>
@@ -499,7 +518,7 @@
                   <c:v>1.8E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2000000000000001E-3</c:v>
+                  <c:v>2.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>4.0000000000000001E-3</c:v>
@@ -511,6 +530,258 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-29DC-43D6-9D7E-2BF6B7887A94}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Raw</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.37899331441159839"/>
+                  <c:y val="-0.24977512044505923"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="20000"/>
+                    <a:lumOff val="80000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-AR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Impact Pipe'!$B$2:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Impact Pipe'!$E$2:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>7.0800000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5700000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0800000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8400000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7799999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.07E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.9000000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4000000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.06E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.4000000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.1000000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.8E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5A9E-491E-AB92-2397FAE5B750}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -772,6 +1043,969 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Amax</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Particle Size - Microphone</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Envelope</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.40462062742939603"/>
+                  <c:y val="-0.17678387948579119"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="20000"/>
+                    <a:lumOff val="80000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Microphone!$B$2:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Microphone!$F$2:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.42620000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7165999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.181</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.43819999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6635</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25240000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.48759999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5174000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1636</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.31130000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.6899999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.42749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.34499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.4899999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.0400000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.1600000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.4699999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.4300000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.2799999999999994E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BDFF-4FF2-B816-C9155A354E68}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Raw Signal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.40475973367178869"/>
+                  <c:y val="-0.39246883750397038"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="20000"/>
+                    <a:lumOff val="80000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-AR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Microphone!$B$2:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Microphone!$E$2:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.41399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.49199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19889999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.43659999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45229999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.63100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2351</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.39989999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1285</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.63100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.16109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.29780000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.6100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.41970000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.34360000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.1900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.8500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.4499999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.4299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.2200000000000004E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3634-4DF1-8D75-78E5E871DF19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="299639312"/>
+        <c:axId val="299627312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="299639312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Diameter</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299627312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="299627312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Max Amplitude</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299639312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -817,12 +2051,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -1372,6 +2640,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1393,6 +3177,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{308EE4C1-EB4A-4103-8986-D8712A8C1056}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>160974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FC5F572-54DF-4884-8642-BB59FE6AF149}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1680,22 +3507,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1709,7 +3536,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1718,7 +3548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>167</v>
       </c>
@@ -1733,6 +3563,9 @@
       </c>
       <c r="E2" s="1">
         <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8.3199999999999996E-2</v>
       </c>
       <c r="G2" s="1">
         <f>D2-C2</f>
@@ -1750,7 +3583,7 @@
         <v>34.347826086956523</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>6</v>
       </c>
@@ -1765,6 +3598,9 @@
       </c>
       <c r="E3" s="1">
         <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3.7100000000000001E-2</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G25" si="1">D3-C3</f>
@@ -1775,7 +3611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -1790,6 +3626,9 @@
       </c>
       <c r="E4" s="1">
         <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.10489999999999999</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="1"/>
@@ -1800,7 +3639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>168</v>
       </c>
@@ -1815,6 +3654,9 @@
       </c>
       <c r="E5" s="1">
         <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4.0300000000000002E-2</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
@@ -1825,7 +3667,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>150</v>
       </c>
@@ -1840,6 +3682,9 @@
       </c>
       <c r="E6" s="1">
         <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.86E-2</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
@@ -1850,7 +3695,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>11</v>
       </c>
@@ -1865,6 +3710,9 @@
       </c>
       <c r="E7" s="1">
         <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.86E-2</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="1"/>
@@ -1875,7 +3723,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>22</v>
       </c>
@@ -1890,6 +3738,9 @@
       </c>
       <c r="E8" s="1">
         <v>2.7799999999999998E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3.0099999999999998E-2</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
@@ -1900,7 +3751,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>152</v>
       </c>
@@ -1915,6 +3766,9 @@
       </c>
       <c r="E9" s="1">
         <v>4.4900000000000002E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4.6800000000000001E-2</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="1"/>
@@ -1925,7 +3779,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>12</v>
       </c>
@@ -1940,6 +3794,9 @@
       </c>
       <c r="E10" s="1">
         <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.9499999999999998E-2</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
@@ -1950,7 +3807,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>96</v>
       </c>
@@ -1965,6 +3822,9 @@
       </c>
       <c r="E11" s="1">
         <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
@@ -1975,7 +3835,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>101</v>
       </c>
@@ -1989,6 +3849,9 @@
         <v>438</v>
       </c>
       <c r="E12" s="1">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="F12" s="1">
         <v>1.4800000000000001E-2</v>
       </c>
       <c r="G12" s="1">
@@ -2000,7 +3863,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>24</v>
       </c>
@@ -2015,6 +3878,9 @@
       </c>
       <c r="E13" s="1">
         <v>4.07E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4.5900000000000003E-2</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
@@ -2025,7 +3891,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>107</v>
       </c>
@@ -2040,6 +3906,9 @@
       </c>
       <c r="E14" s="1">
         <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.9800000000000002E-2</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
@@ -2050,7 +3919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>162</v>
       </c>
@@ -2065,6 +3934,9 @@
       </c>
       <c r="E15" s="1">
         <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.54E-2</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
@@ -2075,7 +3947,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>159</v>
       </c>
@@ -2089,6 +3961,9 @@
         <v>610</v>
       </c>
       <c r="E16" s="1">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="F16" s="1">
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="G16" s="1">
@@ -2100,7 +3975,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>35</v>
       </c>
@@ -2115,6 +3990,9 @@
       </c>
       <c r="E17" s="1">
         <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.03E-2</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="1"/>
@@ -2125,7 +4003,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>69</v>
       </c>
@@ -2140,6 +4018,9 @@
       </c>
       <c r="E18" s="1">
         <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4.7000000000000002E-3</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="1"/>
@@ -2150,7 +4031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>85</v>
       </c>
@@ -2165,6 +4046,9 @@
       </c>
       <c r="E19" s="1">
         <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="1"/>
@@ -2175,7 +4059,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>61</v>
       </c>
@@ -2189,6 +4073,9 @@
         <v>788</v>
       </c>
       <c r="E20" s="1">
+        <v>1.06E-2</v>
+      </c>
+      <c r="F20" s="1">
         <v>1.06E-2</v>
       </c>
       <c r="G20" s="1">
@@ -2200,7 +4087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>52</v>
       </c>
@@ -2215,6 +4102,9 @@
       </c>
       <c r="E21" s="1">
         <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F21" s="1">
+        <v>6.3E-3</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="1"/>
@@ -2225,7 +4115,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>165</v>
       </c>
@@ -2239,6 +4129,9 @@
         <v>875</v>
       </c>
       <c r="E22" s="1">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="F22" s="1">
         <v>5.1000000000000004E-3</v>
       </c>
       <c r="G22" s="1">
@@ -2250,7 +4143,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>166</v>
       </c>
@@ -2264,6 +4157,9 @@
         <v>930</v>
       </c>
       <c r="E23" s="1">
+        <v>1.8E-3</v>
+      </c>
+      <c r="F23" s="1">
         <v>1.8E-3</v>
       </c>
       <c r="G23" s="1">
@@ -2275,7 +4171,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>53</v>
       </c>
@@ -2290,6 +4186,9 @@
       </c>
       <c r="E24" s="1">
         <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2.3E-3</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="1"/>
@@ -2300,7 +4199,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45</v>
       </c>
@@ -2314,6 +4213,9 @@
         <v>1030</v>
       </c>
       <c r="E25" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F25" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G25" s="1">
@@ -2329,20 +4231,943 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160EE506-11C9-432A-9FE1-D04D59569C0D}">
+  <dimension ref="A1:Q27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>167</v>
+      </c>
+      <c r="B2" s="2">
+        <v>128</v>
+      </c>
+      <c r="C2" s="1">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.42620000000000002</v>
+      </c>
+      <c r="G2" s="1">
+        <f>D2-C2</f>
+        <v>25</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" ref="H2:H24" si="0">C3-D2</f>
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(H2:H24)</f>
+        <v>26.913043478260871</v>
+      </c>
+      <c r="P2">
+        <f>C2-'Impact Pipe'!C2</f>
+        <v>9</v>
+      </c>
+      <c r="Q2">
+        <f>D2-'Impact Pipe'!D2</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>128</v>
+      </c>
+      <c r="C3" s="1">
+        <v>90</v>
+      </c>
+      <c r="D3" s="1">
+        <v>110</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G25" si="1">D3-C3</f>
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P3">
+        <f>C3-'Impact Pipe'!C3</f>
+        <v>10</v>
+      </c>
+      <c r="Q3">
+        <f>D3-'Impact Pipe'!D3</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>128</v>
+      </c>
+      <c r="C4" s="1">
+        <v>130</v>
+      </c>
+      <c r="D4" s="1">
+        <v>140</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.7165999999999999</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P4">
+        <f>C4-'Impact Pipe'!C4</f>
+        <v>15</v>
+      </c>
+      <c r="Q4">
+        <f>D4-'Impact Pipe'!D4</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>168</v>
+      </c>
+      <c r="B5" s="2">
+        <v>128</v>
+      </c>
+      <c r="C5" s="1">
+        <v>165</v>
+      </c>
+      <c r="D5" s="1">
+        <v>180</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.181</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P5">
+        <f>C5-'Impact Pipe'!C5</f>
+        <v>15</v>
+      </c>
+      <c r="Q5">
+        <f>D5-'Impact Pipe'!D5</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>150</v>
+      </c>
+      <c r="B6" s="3">
+        <v>90</v>
+      </c>
+      <c r="C6" s="1">
+        <v>200</v>
+      </c>
+      <c r="D6" s="1">
+        <v>215</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.19889999999999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.21290000000000001</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P6">
+        <f>C6-'Impact Pipe'!C6</f>
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <f>D6-'Impact Pipe'!D6</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>90</v>
+      </c>
+      <c r="C7" s="1">
+        <v>240</v>
+      </c>
+      <c r="D7" s="1">
+        <v>250</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.43659999999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.43819999999999998</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P7">
+        <f>C7-'Impact Pipe'!C7</f>
+        <v>14</v>
+      </c>
+      <c r="Q7">
+        <f>D7-'Impact Pipe'!D7</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3">
+        <v>90</v>
+      </c>
+      <c r="C8" s="1">
+        <v>280</v>
+      </c>
+      <c r="D8" s="1">
+        <v>286</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.45229999999999998</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.6008</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="P8">
+        <f>C8-'Impact Pipe'!C8</f>
+        <v>15</v>
+      </c>
+      <c r="Q8">
+        <f>D8-'Impact Pipe'!D8</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>152</v>
+      </c>
+      <c r="B9" s="3">
+        <v>90</v>
+      </c>
+      <c r="C9" s="1">
+        <v>325</v>
+      </c>
+      <c r="D9" s="1">
+        <v>335</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.6635</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P9">
+        <f>C9-'Impact Pipe'!C9</f>
+        <v>15</v>
+      </c>
+      <c r="Q9">
+        <f>D9-'Impact Pipe'!D9</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>64</v>
+      </c>
+      <c r="C10" s="1">
+        <v>365</v>
+      </c>
+      <c r="D10" s="1">
+        <v>375</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.2351</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.25240000000000001</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P10">
+        <f>C10-'Impact Pipe'!C10</f>
+        <v>8</v>
+      </c>
+      <c r="Q10">
+        <f>D10-'Impact Pipe'!D10</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>96</v>
+      </c>
+      <c r="B11" s="4">
+        <v>64</v>
+      </c>
+      <c r="C11" s="1">
+        <v>400</v>
+      </c>
+      <c r="D11" s="1">
+        <v>415</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.39989999999999998</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.48759999999999998</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P11">
+        <f>C11-'Impact Pipe'!C11</f>
+        <v>8</v>
+      </c>
+      <c r="Q11">
+        <f>D11-'Impact Pipe'!D11</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>101</v>
+      </c>
+      <c r="B12" s="4">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1">
+        <v>445</v>
+      </c>
+      <c r="D12" s="1">
+        <v>450</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.1285</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="P12">
+        <f>C12-'Impact Pipe'!C12</f>
+        <v>13</v>
+      </c>
+      <c r="Q12">
+        <f>D12-'Impact Pipe'!D12</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1">
+        <v>485</v>
+      </c>
+      <c r="D13" s="1">
+        <v>490</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.5174000000000001</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P13">
+        <f>C13-'Impact Pipe'!C13</f>
+        <v>17</v>
+      </c>
+      <c r="Q13">
+        <f>D13-'Impact Pipe'!D13</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>107</v>
+      </c>
+      <c r="B14" s="5">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1">
+        <v>520</v>
+      </c>
+      <c r="D14" s="1">
+        <v>540</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.16109999999999999</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.1636</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P14">
+        <f>C14-'Impact Pipe'!C14</f>
+        <v>5</v>
+      </c>
+      <c r="Q14">
+        <f>D14-'Impact Pipe'!D14</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>162</v>
+      </c>
+      <c r="B15" s="5">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1">
+        <v>570</v>
+      </c>
+      <c r="D15" s="1">
+        <v>575</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.29780000000000001</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.31130000000000002</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="P15">
+        <f>C15-'Impact Pipe'!C15</f>
+        <v>20</v>
+      </c>
+      <c r="Q15">
+        <f>D15-'Impact Pipe'!D15</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>159</v>
+      </c>
+      <c r="B16" s="5">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1">
+        <v>610</v>
+      </c>
+      <c r="D16" s="1">
+        <v>625</v>
+      </c>
+      <c r="E16" s="1">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P16">
+        <f>C16-'Impact Pipe'!C16</f>
+        <v>15</v>
+      </c>
+      <c r="Q16">
+        <f>D16-'Impact Pipe'!D16</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>35</v>
+      </c>
+      <c r="B17" s="5">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1">
+        <v>655</v>
+      </c>
+      <c r="D17" s="1">
+        <v>665</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.41970000000000002</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.42749999999999999</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P17">
+        <f>C17-'Impact Pipe'!C17</f>
+        <v>13</v>
+      </c>
+      <c r="Q17">
+        <f>D17-'Impact Pipe'!D17</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>69</v>
+      </c>
+      <c r="B18" s="6">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1">
+        <v>695</v>
+      </c>
+      <c r="D18" s="1">
+        <v>710</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.34360000000000002</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P18">
+        <f>C18-'Impact Pipe'!C18</f>
+        <v>10</v>
+      </c>
+      <c r="Q18">
+        <f>D18-'Impact Pipe'!D18</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>85</v>
+      </c>
+      <c r="B19" s="6">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1">
+        <v>740</v>
+      </c>
+      <c r="D19" s="1">
+        <v>760</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5.1900000000000002E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>6.4899999999999999E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="P19">
+        <f>C19-'Impact Pipe'!C19</f>
+        <v>10</v>
+      </c>
+      <c r="Q19">
+        <f>D19-'Impact Pipe'!D19</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>61</v>
+      </c>
+      <c r="B20" s="6">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1">
+        <v>795</v>
+      </c>
+      <c r="D20" s="1">
+        <v>805</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.1132</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.1132</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P20">
+        <f>C20-'Impact Pipe'!C20</f>
+        <v>13</v>
+      </c>
+      <c r="Q20">
+        <f>D20-'Impact Pipe'!D20</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>52</v>
+      </c>
+      <c r="B21" s="6">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1">
+        <v>830</v>
+      </c>
+      <c r="D21" s="1">
+        <v>850</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
+        <f>C22-D21</f>
+        <v>20</v>
+      </c>
+      <c r="P21">
+        <f>C21-'Impact Pipe'!C21</f>
+        <v>10</v>
+      </c>
+      <c r="Q21">
+        <f>D21-'Impact Pipe'!D21</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>165</v>
+      </c>
+      <c r="B22" s="7">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1">
+        <v>870</v>
+      </c>
+      <c r="D22" s="1">
+        <v>900</v>
+      </c>
+      <c r="E22" s="1">
+        <v>7.4499999999999997E-2</v>
+      </c>
+      <c r="F22" s="1">
+        <v>8.1600000000000006E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <f>D22-C22</f>
+        <v>30</v>
+      </c>
+      <c r="H22" s="1">
+        <f>C23-D22</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>166</v>
+      </c>
+      <c r="B23" s="7">
+        <v>16</v>
+      </c>
+      <c r="C23" s="1">
+        <v>920</v>
+      </c>
+      <c r="D23" s="1">
+        <v>950</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4.4299999999999999E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4.4699999999999997E-2</v>
+      </c>
+      <c r="G23" s="1">
+        <f>D23-C23</f>
+        <v>30</v>
+      </c>
+      <c r="H23" s="1">
+        <f>C24-D23</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>53</v>
+      </c>
+      <c r="B24" s="8">
+        <v>22.6</v>
+      </c>
+      <c r="C24" s="1">
+        <v>970</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E24" s="1">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>5.4300000000000001E-2</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P24">
+        <f>MIN(P2:P22)</f>
+        <v>5</v>
+      </c>
+      <c r="Q24">
+        <f>MIN(Q2:Q22)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45</v>
+      </c>
+      <c r="B25" s="8">
+        <v>22.6</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1020</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1050</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9.2200000000000004E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="P25">
+        <f>AVERAGE(P2:P22)</f>
+        <v>12.05</v>
+      </c>
+      <c r="Q25">
+        <f>AVERAGE(Q2:Q22)</f>
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <f>MEDIAN(P2:P21)</f>
+        <v>13</v>
+      </c>
+      <c r="Q26">
+        <f>MEDIAN(Q2:Q21)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P27">
+        <f>MAX(P2:P21)</f>
+        <v>20</v>
+      </c>
+      <c r="Q27">
+        <f>MAX(Q2:Q21)</f>
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1036A414-1109-4572-9B8B-8712D66EE434}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection sqref="A1:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2353,7 +5178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>167</v>
       </c>
@@ -2364,7 +5189,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>6</v>
       </c>
@@ -2375,7 +5200,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -2386,7 +5211,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>168</v>
       </c>
@@ -2397,7 +5222,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>150</v>
       </c>
@@ -2408,7 +5233,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>11</v>
       </c>
@@ -2419,7 +5244,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>22</v>
       </c>
@@ -2430,7 +5255,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>152</v>
       </c>
@@ -2441,7 +5266,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>12</v>
       </c>
@@ -2452,7 +5277,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>96</v>
       </c>
@@ -2463,7 +5288,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>101</v>
       </c>
@@ -2474,7 +5299,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>24</v>
       </c>
@@ -2485,7 +5310,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>107</v>
       </c>
@@ -2496,7 +5321,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>162</v>
       </c>
@@ -2507,7 +5332,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>159</v>
       </c>
@@ -2518,7 +5343,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>35</v>
       </c>
@@ -2529,7 +5354,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>69</v>
       </c>
@@ -2540,7 +5365,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>85</v>
       </c>
@@ -2551,7 +5376,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>61</v>
       </c>
@@ -2562,7 +5387,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>52</v>
       </c>
@@ -2573,7 +5398,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>165</v>
       </c>
@@ -2584,7 +5409,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>166</v>
       </c>
@@ -2595,7 +5420,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>53</v>
       </c>
@@ -2606,7 +5431,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45</v>
       </c>
@@ -2615,6 +5440,296 @@
       </c>
       <c r="C25" s="1">
         <v>1030</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319700DA-7B79-4076-942B-FE916BF2844A}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>167</v>
+      </c>
+      <c r="B2" s="1">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>90</v>
+      </c>
+      <c r="C3" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>130</v>
+      </c>
+      <c r="C4" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>168</v>
+      </c>
+      <c r="B5" s="1">
+        <v>165</v>
+      </c>
+      <c r="C5" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>150</v>
+      </c>
+      <c r="B6" s="1">
+        <v>200</v>
+      </c>
+      <c r="C6" s="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <v>240</v>
+      </c>
+      <c r="C7" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <v>280</v>
+      </c>
+      <c r="C8" s="1">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>152</v>
+      </c>
+      <c r="B9" s="1">
+        <v>325</v>
+      </c>
+      <c r="C9" s="1">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <v>365</v>
+      </c>
+      <c r="C10" s="1">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>96</v>
+      </c>
+      <c r="B11" s="1">
+        <v>400</v>
+      </c>
+      <c r="C11" s="1">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>101</v>
+      </c>
+      <c r="B12" s="1">
+        <v>445</v>
+      </c>
+      <c r="C12" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1">
+        <v>485</v>
+      </c>
+      <c r="C13" s="1">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>107</v>
+      </c>
+      <c r="B14" s="1">
+        <v>520</v>
+      </c>
+      <c r="C14" s="1">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>162</v>
+      </c>
+      <c r="B15" s="1">
+        <v>570</v>
+      </c>
+      <c r="C15" s="1">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>159</v>
+      </c>
+      <c r="B16" s="1">
+        <v>610</v>
+      </c>
+      <c r="C16" s="1">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1">
+        <v>655</v>
+      </c>
+      <c r="C17" s="1">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>69</v>
+      </c>
+      <c r="B18" s="1">
+        <v>695</v>
+      </c>
+      <c r="C18" s="1">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>85</v>
+      </c>
+      <c r="B19" s="1">
+        <v>740</v>
+      </c>
+      <c r="C19" s="1">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>61</v>
+      </c>
+      <c r="B20" s="1">
+        <v>795</v>
+      </c>
+      <c r="C20" s="1">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1">
+        <v>830</v>
+      </c>
+      <c r="C21" s="1">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>165</v>
+      </c>
+      <c r="B22" s="1">
+        <v>870</v>
+      </c>
+      <c r="C22" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>166</v>
+      </c>
+      <c r="B23" s="1">
+        <v>920</v>
+      </c>
+      <c r="C23" s="1">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>53</v>
+      </c>
+      <c r="B24" s="1">
+        <v>970</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1020</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished processing the hydrophones (for now)
</commit_message>
<xml_diff>
--- a/Hydrophones/Calibration/ManualRockMovements-1/mov1_calibration_curve.xlsx
+++ b/Hydrophones/Calibration/ManualRockMovements-1/mov1_calibration_curve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Hydrophones\Calibration\ManualRockMovements-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E51FE61-EC7D-4045-B64B-90704AA31749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5402F2A4-60C3-4456-B270-80B0258BA28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3508,7 +3508,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="E2" sqref="E2:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4235,7 +4235,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>